<commit_message>
Tests were performed for point-point icp and point-plane icp
</commit_message>
<xml_diff>
--- a/RegistrationResults/Filtered fit RMSE.xlsx
+++ b/RegistrationResults/Filtered fit RMSE.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,198 +437,283 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Test#</t>
+          <t>One Room RANSAC</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>One Room</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Two Rooms</t>
+          <t>One Room Refined</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Three Rooms</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Four Rooms</t>
+          <t>Two Rooms RANSAC</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Two Rooms Refined</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Three Rooms RANSAC</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Three Rooms Refined</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Four Rooms RANSAC</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Four Rooms Refined</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0.2518898123372789</v>
       </c>
       <c r="B2" t="n">
-        <v>0.140649720169261</v>
+        <v>0.1000039577484131</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1356531242717383</v>
+        <v>0.1482372422167708</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1382637833234396</v>
+        <v>0.05199837684631348</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1370295539762188</v>
+        <v>0.2261681963224231</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0800025463104248</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1633780183892594</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02500176429748535</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.2436729525948772</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1100020408630371</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1473568526337741</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.1060006618499756</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.2061270982166633</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.09900116920471191</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.1458469042296603</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.09400224685668945</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>0.2764373150518605</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1223045497581388</v>
+        <v>0.1010017395019531</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1334553413460124</v>
+        <v>0.1472837945855425</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1364462720148708</v>
+        <v>0.02199602127075195</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1354067427513968</v>
+        <v>0.2604920049314019</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.09000301361083984</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1633779939964034</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.03400063514709473</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.3047929911143028</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.1120002269744873</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.1473565875268908</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.1149978637695312</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.2250521677412161</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.104001522064209</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.1458469768804727</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.1719973087310791</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>0.3498953023264292</v>
       </c>
       <c r="B4" t="n">
-        <v>0.136606025885821</v>
+        <v>0.1089985370635986</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1319316064950641</v>
+        <v>0.1589493327675606</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1342212127005677</v>
+        <v>0.05099797248840332</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1340554966890002</v>
+        <v>0.2236084222637152</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.08100247383117676</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1629723345984794</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.03000020980834961</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.218573030925764</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1090028285980225</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.1474637758030676</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.1060028076171875</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.2463742064013847</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.09799885749816895</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.1458469768149112</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.1659984588623047</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>0.3001472564275787</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1967234276928571</v>
+        <v>0.1019971370697021</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1309813334370294</v>
+        <v>0.1482372422167708</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1319211917553566</v>
+        <v>0.0579979419708252</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1327044361041245</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.1331664369924049</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1299623188498496</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1303635958465269</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.1320048897653829</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.1936853376081075</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1293726403860927</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.1286711625090799</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.1315602081645383</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.1978117409176318</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.1283776424146626</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.1281102867183086</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1302692371737562</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.1961268317314818</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.1278627948587868</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.1280102546796128</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.1299377218199589</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.1991934188172659</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.1276269261710007</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.1279158522964733</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.1294667057285463</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.1989204540907865</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.1275556592551687</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.1276172175192556</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.1286527082860713</v>
+        <v>0.2624189214276322</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.08099794387817383</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1629725749536803</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.03200197219848633</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.2185730309257643</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1140010356903076</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1474637758030677</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1010012626647949</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1981651280651061</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1120011806488037</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.1458472395410905</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.1030004024505615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>